<commit_message>
support more gameplay effect export and import functions.
</commit_message>
<xml_diff>
--- a/Plugins/AbilityEditorHelper/DataSample/Test.xlsx
+++ b/Plugins/AbilityEditorHelper/DataSample/Test.xlsx
@@ -4,11 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29868" windowHeight="12780"/>
+    <workbookView windowWidth="29868" windowHeight="12780" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GameplayEffectConfig" sheetId="1" r:id="rId1"/>
     <sheet name="GameplayEffectConfig.Modifiers" sheetId="2" r:id="rId2"/>
+    <sheet name="GameplayEffectConfig.GameplayCu" sheetId="3" r:id="rId3"/>
+    <sheet name="GameplayEffectConfig.ImmunityQu" sheetId="4" r:id="rId4"/>
+    <sheet name="GameplayEffectConfig.RemovalQue" sheetId="5" r:id="rId5"/>
+    <sheet name="GameplayEffectConfig.Executions" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,11 +32,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>ParentClass</t>
+  </si>
+  <si>
     <t>DurationType</t>
   </si>
   <si>
@@ -60,9 +67,27 @@
     <t>GrantedTags</t>
   </si>
   <si>
+    <t>ApplicationTagRequirements</t>
+  </si>
+  <si>
+    <t>OngoingTagRequirements</t>
+  </si>
+  <si>
+    <t>RemovalTagRequirements</t>
+  </si>
+  <si>
+    <t>CancelAbilitiesWithTags</t>
+  </si>
+  <si>
+    <t>BlockAbilitiesWithTags</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
+    <t>Asset path: /Game/Effects/GE_Base</t>
+  </si>
+  <si>
     <t>Instant | Infinite | HasDuration</t>
   </si>
   <si>
@@ -78,7 +103,7 @@
     <t>用逗号/分号分隔：TagA, TagB.Sub</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>Test1</t>
   </si>
   <si>
     <t>Instant</t>
@@ -108,6 +133,21 @@
     <t>Magnitude</t>
   </si>
   <si>
+    <t>AttributeBasedConfig</t>
+  </si>
+  <si>
+    <t>SetByCallerConfig</t>
+  </si>
+  <si>
+    <t>CustomCalculationClass</t>
+  </si>
+  <si>
+    <t>SourceTagRequirements</t>
+  </si>
+  <si>
+    <t>TargetTagRequirements</t>
+  </si>
+  <si>
     <t>格式：/Script/Module.Class:Property</t>
   </si>
   <si>
@@ -117,13 +157,43 @@
     <t>ScalableFloat | AttributeBased | CustomCalculationClass | SetByCaller</t>
   </si>
   <si>
-    <t>/Script/GameplayAbilities.AbilitySystemComponent:OutgoingDuration</t>
-  </si>
-  <si>
-    <t>AddBase</t>
-  </si>
-  <si>
-    <t>ScalableFloat</t>
+    <t>Asset path to calculation class</t>
+  </si>
+  <si>
+    <t>GameplayCueTag</t>
+  </si>
+  <si>
+    <t>MinLevel</t>
+  </si>
+  <si>
+    <t>MaxLevel</t>
+  </si>
+  <si>
+    <t>MatchAnyOwningTags</t>
+  </si>
+  <si>
+    <t>MatchAllOwningTags</t>
+  </si>
+  <si>
+    <t>MatchNoOwningTags</t>
+  </si>
+  <si>
+    <t>MatchAnySourceTags</t>
+  </si>
+  <si>
+    <t>MatchAllSourceTags</t>
+  </si>
+  <si>
+    <t>MatchNoSourceTags</t>
+  </si>
+  <si>
+    <t>CalculationClass</t>
+  </si>
+  <si>
+    <t>PassedInTags</t>
+  </si>
+  <si>
+    <t>Asset path to execution calculation class</t>
   </si>
 </sst>
 </file>
@@ -1092,25 +1162,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2"/>
   <cols>
-    <col min="2" max="2" width="33.7777777777778" customWidth="1"/>
-    <col min="3" max="3" width="30.3333333333333" customWidth="1"/>
-    <col min="5" max="5" width="23.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="26.2222222222222" customWidth="1"/>
-    <col min="7" max="7" width="39.6666666666667" customWidth="1"/>
-    <col min="8" max="8" width="33.5555555555556" customWidth="1"/>
-    <col min="9" max="9" width="16.3333333333333" customWidth="1"/>
-    <col min="10" max="10" width="20.5555555555556" customWidth="1"/>
+    <col min="2" max="2" width="24.7777777777778" customWidth="1"/>
+    <col min="3" max="3" width="18.2222222222222" customWidth="1"/>
+    <col min="4" max="4" width="19.1111111111111" customWidth="1"/>
+    <col min="8" max="8" width="23.2222222222222" customWidth="1"/>
+    <col min="9" max="9" width="34.3333333333333" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="16.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1141,63 +1210,96 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1209,69 +1311,286 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="4"/>
-  <cols>
-    <col min="2" max="2" width="75.2222222222222" customWidth="1"/>
-    <col min="3" max="3" width="29.4444444444444" customWidth="1"/>
-    <col min="4" max="4" width="30.6666666666667" customWidth="1"/>
-    <col min="5" max="5" width="23.7777777777778" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>22</v>
       </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>